<commit_message>
fix POMBOX labels (#64)
</commit_message>
<xml_diff>
--- a/submissions/browse-article-28244182/submission.xlsx
+++ b/submissions/browse-article-28244182/submission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Manu/Documents/Projects/ShareYourCloning/ShareYourCloning-submission/submissions/browse-article-28244182/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49AC477-4C11-624C-AA92-F35EB202172B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E681BA-A009-4345-B85E-0119CCF03516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13840" yWindow="500" windowWidth="27480" windowHeight="21460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="500" windowWidth="27480" windowHeight="21460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequence" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{B8E1B018-3713-E44C-A24C-7A204504DBAB}" name="plasmids (1)" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/Manu/Downloads/plasmids (1).tsv" decimal="," thousands=".">
+    <textPr sourceFile="/Users/Manu/Downloads/plasmids (1).tsv" decimal="," thousands=".">
       <textFields count="6">
         <textField type="text"/>
         <textField/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="372">
   <si>
     <t>name</t>
   </si>
@@ -262,22 +262,13 @@
     <t>7h</t>
   </si>
   <si>
-    <t>3''his5</t>
-  </si>
-  <si>
     <t>pPOM040_P8b_5'Ura4</t>
   </si>
   <si>
     <t>8b</t>
   </si>
   <si>
-    <t>5'ura4</t>
-  </si>
-  <si>
     <t>pPOM036_P7_3"Ura4</t>
-  </si>
-  <si>
-    <t>3''ura4</t>
   </si>
   <si>
     <t>id</t>
@@ -1152,6 +1143,27 @@
   <si>
     <t>https://www.addgene.org/kits/pluskal-pombox/#kit-contents</t>
   </si>
+  <si>
+    <t>ConL1</t>
+  </si>
+  <si>
+    <t>ConL2</t>
+  </si>
+  <si>
+    <t>ConL3</t>
+  </si>
+  <si>
+    <t>3'Lys3</t>
+  </si>
+  <si>
+    <t>3'Ura4</t>
+  </si>
+  <si>
+    <t>5'Lys3</t>
+  </si>
+  <si>
+    <t>5'Ura4</t>
+  </si>
 </sst>
 </file>
 
@@ -1502,7 +1514,7 @@
   <dimension ref="A1:J105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1552,10 +1564,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>7</v>
@@ -1574,10 +1586,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>9</v>
@@ -1596,10 +1608,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>11</v>
@@ -1618,10 +1630,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>13</v>
@@ -1640,10 +1652,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>15</v>
@@ -1662,10 +1674,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>17</v>
@@ -1684,10 +1696,10 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>19</v>
@@ -1706,10 +1718,10 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>21</v>
@@ -1728,10 +1740,10 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E10" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>23</v>
@@ -1750,10 +1762,10 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E11" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>25</v>
@@ -1772,10 +1784,10 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>27</v>
@@ -1794,10 +1806,10 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>29</v>
@@ -1816,10 +1828,10 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E14" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>31</v>
@@ -1838,10 +1850,10 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E15" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>33</v>
@@ -1860,10 +1872,10 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E16" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>35</v>
@@ -1882,10 +1894,10 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E17" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>37</v>
@@ -1904,10 +1916,10 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E18" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>39</v>
@@ -1926,10 +1938,10 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E19" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>41</v>
@@ -1948,10 +1960,10 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E20" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>43</v>
@@ -1970,10 +1982,10 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E21" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>45</v>
@@ -1992,10 +2004,10 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E22" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>47</v>
@@ -2014,10 +2026,10 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E23" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>49</v>
@@ -2036,10 +2048,10 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E24" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>51</v>
@@ -2058,10 +2070,10 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E25" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>53</v>
@@ -2080,10 +2092,10 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E26" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>55</v>
@@ -2102,10 +2114,10 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>57</v>
@@ -2124,10 +2136,10 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E28" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>59</v>
@@ -2146,10 +2158,10 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E29" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>61</v>
@@ -2168,10 +2180,10 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E30" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>63</v>
@@ -2190,10 +2202,10 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E31" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>65</v>
@@ -2212,10 +2224,10 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E32" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>67</v>
@@ -2233,10 +2245,10 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E33" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>69</v>
@@ -2245,7 +2257,7 @@
     </row>
     <row r="34" spans="1:8" ht="13">
       <c r="A34" s="19" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B34">
         <v>216459</v>
@@ -2254,19 +2266,19 @@
         <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E34" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>71</v>
+        <v>368</v>
       </c>
       <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" ht="13">
       <c r="A35" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B35">
         <v>216465</v>
@@ -2275,1153 +2287,1161 @@
         <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E35" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>74</v>
+        <v>369</v>
       </c>
       <c r="H35" s="19"/>
     </row>
     <row r="36" spans="1:8" ht="13">
       <c r="A36" s="19" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B36">
         <v>216463</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D36" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E36" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>76</v>
+        <v>370</v>
       </c>
       <c r="H36" s="19"/>
     </row>
     <row r="37" spans="1:8" ht="13">
       <c r="A37" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37">
         <v>216461</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D37" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E37" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>146</v>
+        <v>371</v>
       </c>
       <c r="H37" s="19"/>
     </row>
     <row r="38" spans="1:8" ht="13">
       <c r="A38" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C38" s="5">
         <v>1</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="13">
       <c r="A39" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C39" s="5">
         <v>1</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>163</v>
+        <v>365</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="13">
       <c r="A40" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C40" s="5">
         <v>1</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>167</v>
+        <v>366</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="13">
       <c r="A41" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C41" s="5">
         <v>1</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>171</v>
+        <v>367</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="13">
       <c r="A42" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C42" s="5">
         <v>1</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="13">
       <c r="A43" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C43" s="5">
         <v>1</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="13">
       <c r="A44" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C44" s="5">
         <v>1</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="13">
       <c r="A45" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C45" s="5">
         <v>3</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="13">
       <c r="A46" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C46" s="5">
         <v>3</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="13">
       <c r="A47" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C47" s="5">
         <v>3</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="13">
       <c r="A48" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C48" s="5">
         <v>3</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="13">
       <c r="A49" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="13">
       <c r="A50" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="13">
       <c r="A51" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="13">
       <c r="A52" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="13">
       <c r="A53" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="13">
       <c r="A54" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="13">
       <c r="A55" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>221</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="13">
       <c r="A56" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F56" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="13">
       <c r="A57" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C57" s="5">
         <v>234</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="13">
       <c r="A58" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C58" s="5">
         <v>234</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="13">
       <c r="A59" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C59" s="5">
         <v>4</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="13">
       <c r="A60" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C60" s="5">
         <v>4</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="13">
       <c r="A61" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C61" s="5">
         <v>4</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>171</v>
+        <v>226</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="13">
       <c r="A62" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C62" s="5">
         <v>4</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>175</v>
+        <v>230</v>
       </c>
       <c r="H62" s="19"/>
     </row>
     <row r="63" spans="1:8" ht="13">
       <c r="A63" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C63" s="5">
         <v>4</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>179</v>
+        <v>234</v>
       </c>
       <c r="H63" s="19"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1">
       <c r="A64" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C64" s="5">
         <v>4</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>196</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="13">
       <c r="A65" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>221</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="13">
       <c r="A66" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>225</v>
+        <v>172</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="13">
       <c r="A67" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>229</v>
+        <v>176</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="13">
       <c r="A68" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>233</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="13">
       <c r="A69" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="J69" s="19"/>
     </row>
     <row r="70" spans="1:10" ht="13">
       <c r="A70" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="J70" s="19"/>
     </row>
     <row r="71" spans="1:10" ht="13">
       <c r="A71" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>275</v>
+        <v>226</v>
       </c>
       <c r="J71" s="19"/>
     </row>
     <row r="72" spans="1:10" ht="13">
       <c r="A72" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>279</v>
+        <v>230</v>
       </c>
       <c r="J72" s="19"/>
     </row>
     <row r="73" spans="1:10" ht="13">
       <c r="A73" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>283</v>
+        <v>234</v>
       </c>
       <c r="J73" s="19"/>
     </row>
     <row r="74" spans="1:10" ht="13">
       <c r="A74" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>287</v>
+        <v>238</v>
       </c>
       <c r="J74" s="19"/>
     </row>
     <row r="75" spans="1:10" ht="13">
       <c r="A75" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C75" s="5">
         <v>5</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="J75" s="19"/>
     </row>
     <row r="76" spans="1:10" ht="13">
       <c r="A76" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C76" s="5">
         <v>5</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="J76" s="19"/>
     </row>
     <row r="77" spans="1:10" ht="13">
       <c r="A77" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C77" s="5">
         <v>5</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="J77" s="19"/>
     </row>
     <row r="78" spans="1:10" ht="13">
       <c r="A78" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C78" s="5">
         <v>5</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="J78" s="19"/>
     </row>
     <row r="79" spans="1:10" ht="13">
       <c r="A79" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C79" s="5">
         <v>5</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="J79" s="19"/>
     </row>
     <row r="80" spans="1:10" ht="13">
       <c r="A80" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C80" s="5">
         <v>5</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
       <c r="J80" s="19"/>
     </row>
     <row r="81" spans="1:10" ht="13">
       <c r="A81" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C81" s="5">
         <v>5</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="J81" s="19"/>
     </row>
     <row r="82" spans="1:10" ht="13">
       <c r="A82" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C82" s="5">
         <v>6</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="J82" s="19"/>
     </row>
     <row r="83" spans="1:10" ht="13">
       <c r="A83" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C83" s="5">
         <v>6</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="J83" s="19"/>
     </row>
     <row r="84" spans="1:10" ht="13">
       <c r="A84" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C84" s="5">
         <v>6</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
       <c r="J84" s="19"/>
     </row>
     <row r="85" spans="1:10" ht="13">
       <c r="A85" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C85" s="5">
         <v>6</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="J85" s="19"/>
     </row>
     <row r="86" spans="1:10" ht="13">
       <c r="A86" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C86" s="5">
         <v>8</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="J86" s="19"/>
     </row>
     <row r="87" spans="1:10" ht="13">
       <c r="A87" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C87" s="5">
         <v>8</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="J87" s="19"/>
     </row>
     <row r="88" spans="1:10" ht="13">
       <c r="A88" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C88" s="5">
         <v>8</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="F88" s="6"/>
+        <v>326</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>327</v>
+      </c>
       <c r="J88" s="19"/>
     </row>
     <row r="89" spans="1:10" ht="13">
       <c r="A89" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="F89" s="6"/>
+        <v>330</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="J89" s="19"/>
     </row>
     <row r="90" spans="1:10" ht="13">
       <c r="A90" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="F90" s="6"/>
+        <v>333</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>322</v>
+      </c>
       <c r="J90" s="19"/>
     </row>
     <row r="91" spans="1:10" ht="13">
       <c r="A91" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="F91" s="6"/>
+        <v>336</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>327</v>
+      </c>
       <c r="J91" s="19"/>
     </row>
     <row r="92" spans="1:10" ht="13">
@@ -3519,16 +3539,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -3558,11 +3578,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -3592,11 +3612,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -3626,13 +3646,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -3659,16 +3679,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3695,16 +3715,16 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3731,10 +3751,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -3766,7 +3786,7 @@
         <v>234</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -3798,11 +3818,11 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -3829,16 +3849,16 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -3865,14 +3885,14 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -3902,11 +3922,11 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -3936,11 +3956,11 @@
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -3970,11 +3990,11 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -4004,11 +4024,11 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -4038,11 +4058,11 @@
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -4069,14 +4089,14 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -4103,14 +4123,14 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -31657,13 +31677,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>5</v>
@@ -31671,16 +31691,16 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
@@ -31709,24 +31729,24 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -31752,10 +31772,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>5</v>
@@ -31767,10 +31787,10 @@
         <v>1|2|3|4|5|6|7|8</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
@@ -31779,10 +31799,10 @@
         <v>1|2|3a|3b|4|5|6|7|8</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
@@ -31791,10 +31811,10 @@
         <v>1|2|3a|3b|4a|4b|5|6|7|8</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1">
@@ -31803,10 +31823,10 @@
         <v>1|2|3|4|5|6|7h|8a|8b</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
@@ -31815,10 +31835,10 @@
         <v>1|2|3a|3b|4|5|6|7h|8a|8b</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1">
@@ -31827,10 +31847,10 @@
         <v>1|2|3a|3b|4a|4b|5|6|7h|8a|8b</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1">
@@ -31937,10 +31957,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E2" s="17">
         <v>4</v>
@@ -31983,16 +32003,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G3" s="17">
         <v>5</v>
@@ -32046,10 +32066,10 @@
         <v>70</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
@@ -32077,10 +32097,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E5" s="17">
         <v>4</v>
@@ -32095,10 +32115,10 @@
         <v>70</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="16"/>
@@ -32125,16 +32145,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G6" s="17">
         <v>5</v>
@@ -32146,10 +32166,10 @@
         <v>70</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L6" s="16"/>
       <c r="M6" s="16"/>
@@ -60032,7 +60052,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -60056,10 +60076,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
fix 7h, 8a, 8b glyphs
</commit_message>
<xml_diff>
--- a/submissions/browse-article-28244182/submission.xlsx
+++ b/submissions/browse-article-28244182/submission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Manu/Documents/Projects/ShareYourCloning/ShareYourCloning-submission/submissions/browse-article-28244182/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E681BA-A009-4345-B85E-0119CCF03516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E446D906-654D-644F-B46B-CEBE9CD01838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="500" windowWidth="27480" windowHeight="21460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="500" windowWidth="27480" windowHeight="21460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequence" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="375">
   <si>
     <t>name</t>
   </si>
@@ -1164,6 +1164,15 @@
   <si>
     <t>5'Ura4</t>
   </si>
+  <si>
+    <t>glyph_7h.png</t>
+  </si>
+  <si>
+    <t>glyph_8a.png</t>
+  </si>
+  <si>
+    <t>glyph_8b.png</t>
+  </si>
 </sst>
 </file>
 
@@ -1513,7 +1522,7 @@
   </sheetPr>
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
@@ -3527,8 +3536,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4028,7 +4037,7 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>106</v>
+        <v>372</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -4096,7 +4105,7 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>109</v>
+        <v>373</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -4130,7 +4139,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>109</v>
+        <v>374</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>

</xml_diff>

<commit_message>
fix 7h, 8a, 8b glyphs (#65)
</commit_message>
<xml_diff>
--- a/submissions/browse-article-28244182/submission.xlsx
+++ b/submissions/browse-article-28244182/submission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Manu/Documents/Projects/ShareYourCloning/ShareYourCloning-submission/submissions/browse-article-28244182/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E681BA-A009-4345-B85E-0119CCF03516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E446D906-654D-644F-B46B-CEBE9CD01838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="500" windowWidth="27480" windowHeight="21460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="500" windowWidth="27480" windowHeight="21460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequence" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="375">
   <si>
     <t>name</t>
   </si>
@@ -1164,6 +1164,15 @@
   <si>
     <t>5'Ura4</t>
   </si>
+  <si>
+    <t>glyph_7h.png</t>
+  </si>
+  <si>
+    <t>glyph_8a.png</t>
+  </si>
+  <si>
+    <t>glyph_8b.png</t>
+  </si>
 </sst>
 </file>
 
@@ -1513,7 +1522,7 @@
   </sheetPr>
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
@@ -3527,8 +3536,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4028,7 +4037,7 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>106</v>
+        <v>372</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -4096,7 +4105,7 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>109</v>
+        <v>373</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -4130,7 +4139,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>109</v>
+        <v>374</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>

</xml_diff>